<commit_message>
added error handling at one location, added new task for translating docus
</commit_message>
<xml_diff>
--- a/Task 17 - Templates and Template docus/to_translate.xlsx
+++ b/Task 17 - Templates and Template docus/to_translate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4658" uniqueCount="2283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4666" uniqueCount="2291">
   <si>
     <t xml:space="preserve">title</t>
   </si>
@@ -6873,6 +6873,30 @@
   </si>
   <si>
     <t xml:space="preserve">ويكيپيديا</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قوالب أقاليم المغرب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">موضيلات أقاليم لمغريب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">يُمكن استخدام</t>
+  </si>
+  <si>
+    <t xml:space="preserve">تقدر تخدّم</t>
+  </si>
+  <si>
+    <t xml:space="preserve">وسيط</t>
+  </si>
+  <si>
+    <t xml:space="preserve">پاراميطر</t>
+  </si>
+  <si>
+    <t xml:space="preserve">قوالب جهات المغرب</t>
+  </si>
+  <si>
+    <t xml:space="preserve">موضيلات جهات لمغريب</t>
   </si>
 </sst>
 </file>
@@ -6994,7 +7018,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="19.71"/>
@@ -25051,16 +25075,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.16"/>
   </cols>
   <sheetData>
@@ -25576,6 +25600,38 @@
       </c>
       <c r="C47" s="0" t="s">
         <v>2282</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
+        <v>2283</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>2284</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
+        <v>2285</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>2286</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
+        <v>2287</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>2288</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>2289</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>2290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>